<commit_message>
adding db, change excel
</commit_message>
<xml_diff>
--- a/LIG数据分类.xlsx
+++ b/LIG数据分类.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\ui-code-generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7CA830-CE86-4721-B8E7-BE9C90746008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F005DEE6-2DD0-4786-93A3-CB20723AA651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6E56D278-3853-45EA-AE31-7021E5B052FF}"/>
   </bookViews>
@@ -902,10 +902,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>xxxxxxxx Megawatt-Hours,  1MWH</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>xxxxxxxx Miles, 1 Mile</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1050,6 +1046,10 @@
   </si>
   <si>
     <t>xxxx.x A RMS, 0.1 ARMS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxxxxxxx Megawatt-Hours,  1 MWH</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1537,8 +1537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D944C31-6BEE-494B-9BFA-1345CBD85D16}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C47" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1554,9 +1554,9 @@
     <col min="9" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="5"/>
@@ -1565,7 +1565,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="151.80000000000001" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1666,10 +1666,10 @@
         <v>32</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="147" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>19</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>134</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>36</v>
@@ -1769,7 +1769,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>23</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="172.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>25</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>27</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
@@ -1904,7 +1904,7 @@
       <c r="F15" s="8"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
@@ -1913,7 +1913,7 @@
       <c r="F16" s="8"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
@@ -1924,33 +1924,33 @@
       <c r="F17" s="6"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>153</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>165</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>140</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>40</v>
       </c>
@@ -1961,22 +1961,22 @@
         <v>154</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>166</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>141</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>41</v>
       </c>
@@ -1987,22 +1987,22 @@
         <v>155</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>167</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>184</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>42</v>
       </c>
@@ -2013,22 +2013,22 @@
         <v>156</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>168</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>185</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
@@ -2039,22 +2039,22 @@
         <v>157</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>169</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>186</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
@@ -2065,22 +2065,22 @@
         <v>158</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>170</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>187</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -2091,22 +2091,22 @@
         <v>159</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>171</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>188</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -2117,22 +2117,22 @@
         <v>160</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>135</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>189</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>96</v>
       </c>
@@ -2143,22 +2143,22 @@
         <v>161</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>136</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>190</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>97</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>162</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>137</v>
@@ -2181,21 +2181,21 @@
         <v>191</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>163</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>138</v>
@@ -2207,31 +2207,31 @@
         <v>192</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>164</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>139</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="7"/>
@@ -2240,7 +2240,7 @@
       <c r="F30" s="8"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
@@ -2251,7 +2251,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>98</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>99</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>100</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>101</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>102</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>103</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>104</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>105</v>
       </c>
@@ -2456,10 +2456,10 @@
         <v>183</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>106</v>
       </c>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="7"/>
@@ -2489,7 +2489,7 @@
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>2</v>
       </c>
@@ -2500,7 +2500,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="5"/>
     </row>
-    <row r="43" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>50</v>
       </c>
@@ -2523,10 +2523,10 @@
         <v>175</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>51</v>
       </c>
@@ -2549,10 +2549,10 @@
         <v>176</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>52</v>
       </c>
@@ -2569,16 +2569,16 @@
         <v>147</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>177</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>53</v>
       </c>
@@ -2595,16 +2595,16 @@
         <v>148</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>178</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>54</v>
       </c>
@@ -2621,16 +2621,16 @@
         <v>149</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>179</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>55</v>
       </c>
@@ -2647,16 +2647,16 @@
         <v>150</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>180</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>56</v>
       </c>
@@ -2673,16 +2673,16 @@
         <v>172</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>181</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>57</v>
       </c>
@@ -2699,16 +2699,16 @@
         <v>173</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>182</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>58</v>
       </c>
@@ -2725,11 +2725,11 @@
         <v>174</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>59</v>
       </c>
@@ -2742,7 +2742,7 @@
       <c r="F52" s="8"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="8"/>
       <c r="C53" s="7"/>
@@ -2751,7 +2751,7 @@
       <c r="F53" s="8"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>3</v>
       </c>
@@ -2762,7 +2762,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="5"/>
     </row>
-    <row r="55" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>12</v>
       </c>
@@ -2773,22 +2773,22 @@
         <v>18</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>194</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G55" s="7" t="s">
         <v>200</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>13</v>
       </c>
@@ -2805,16 +2805,16 @@
         <v>195</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>71</v>
@@ -2826,11 +2826,11 @@
         <v>196</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:8" ht="84" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>15</v>
       </c>
@@ -2847,11 +2847,11 @@
         <v>197</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:8" ht="42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>16</v>
       </c>
@@ -2868,11 +2868,11 @@
         <v>198</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>17</v>
       </c>
@@ -2887,11 +2887,11 @@
         <v>199</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="8"/>
       <c r="C61" s="7"/>
@@ -2900,7 +2900,7 @@
       <c r="F61" s="8"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" s="1" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>4</v>
       </c>
@@ -2911,7 +2911,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>74</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="F63" s="8"/>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>75</v>
       </c>
@@ -2941,7 +2941,7 @@
       <c r="F64" s="8"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>76</v>
       </c>
@@ -2956,7 +2956,7 @@
       <c r="F65" s="8"/>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="8"/>
       <c r="C66" s="7"/>

</xml_diff>